<commit_message>
EPBDS-8370 Error "java.lang.IllegalArgumentException: array element type mismatch" is presented on runtime
--HG--
branch : 5.21.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8370.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8370.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C997F610-EB1E-49B9-93C6-6CB73FE539FC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="10800"/>
+    <workbookView xWindow="2055" yWindow="1800" windowWidth="31485" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Step</t>
   </si>
@@ -64,15 +70,9 @@
     <t>Spreadsheet SpreadsheetResult mySpr_good_array()</t>
   </si>
   <si>
-    <t>Spreadsheet SpreadsheetResult mySpr_bag_aray()</t>
-  </si>
-  <si>
     <t>Test mySpr_good_array mySpr_good_arrayTest</t>
   </si>
   <si>
-    <t>_res_</t>
-  </si>
-  <si>
     <t>Result</t>
   </si>
   <si>
@@ -82,37 +82,20 @@
     <t>_res_.$Value$Step4</t>
   </si>
   <si>
-    <t>Test mySpr_good_array mySpr_bad_arrayTest</t>
-  </si>
-  <si>
     <t>Test mySpr_bad_array mySpr_bad_arrayTest</t>
   </si>
   <si>
-    <t>Spreadsheet SpreadsheetResult mySpr_bab_aray()</t>
-  </si>
-  <si>
-    <t>Spreadsheet SpreadsheetResult mySpr_bad_aray()</t>
-  </si>
-  <si>
     <t>Spreadsheet SpreadsheetResult mySpr_bad_array()</t>
   </si>
   <si>
-    <t>7,8,9,10,11,12,1,2,3,1,2,3,4,5,6</t>
+    <t>7,8,9,10,11,12,1,2,3,4,5,6,1,2,3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1" rgb="000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,52 +103,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Franklin Gothic Book"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Franklin Gothic Book"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -189,39 +136,35 @@
       <diagonal/>
     </border>
     <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -272,13 +215,13 @@
     </dxf>
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Table Style 1" pivot="0" count="0"/>
-    <tableStyle name="-History--style" pivot="0" count="3">
+    <tableStyle name="Table Style 1" pivot="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
+    <tableStyle name="-History--style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="headerRow" dxfId="4"/>
       <tableStyleElement type="firstRowStripe" dxfId="3"/>
       <tableStyleElement type="secondRowStripe" dxfId="2"/>
     </tableStyle>
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -287,14 +230,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -332,9 +278,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -367,9 +313,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -402,9 +365,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -577,161 +557,161 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="34.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="30.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="46.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="2" max="2" width="34.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="46" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="G2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="2"/>
+      <c r="C2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13">
-      <c r="B13" t="s" s="5">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14">
-      <c r="B14" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" t="s" s="5">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16">
-      <c r="B16" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" t="s" s="5">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" t="s" s="5">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" t="s" s="5">
-        <v>27</v>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>